<commit_message>
Update Files Banners KOA/KOE
</commit_message>
<xml_diff>
--- a/public/xlsx/koa/BANNERS-MARCAS-KOA-KOE.xlsx
+++ b/public/xlsx/koa/BANNERS-MARCAS-KOA-KOE.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sernar/GITHUB/vmlyr/trade/src/xlsx/koe/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sernar/GITHUB/vmlyr/trade/public/xlsx/koa/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49148A5C-31DA-A849-BE29-18377E719789}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDCD28A3-0253-B14C-BF0C-A0F57EE6A2A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30240" yWindow="3400" windowWidth="27200" windowHeight="14860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -141,7 +141,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="126">
   <si>
     <t>Marca</t>
   </si>
@@ -245,9 +245,6 @@
     <t>#1 MÁS VENDIDA EN ESTADOS UNIDOS</t>
   </si>
   <si>
-    <t>· Fácil de beber, ligera, refrescante y siempre con un sabor superior.</t>
-  </si>
-  <si>
     <t>Coors, Royal Guard</t>
   </si>
   <si>
@@ -374,9 +371,6 @@
     <t>40% MENOS CALORÍAS QUE UNA CERVEZA REGULAR</t>
   </si>
   <si>
-    <t>· Cerveza premium de estilo lager, liviana y refrescante.</t>
-  </si>
-  <si>
     <t>Sol</t>
   </si>
   <si>
@@ -416,9 +410,6 @@
     <t>CERVEZA ARGENTINA</t>
   </si>
   <si>
-    <t>· Cerveza dorada y equilibrada,  hecha con ingredientes naturales de campos argentinos.</t>
-  </si>
-  <si>
     <t>Stella Artois</t>
   </si>
   <si>
@@ -455,32 +446,80 @@
     <t>-</t>
   </si>
   <si>
-    <t>· Conocida como La Baltiloca. · Es la chela del pueblo y una de las más queridas por los chilenos.</t>
-  </si>
-  <si>
-    <t>· 3ra más vendida en Chile. · Premiada por su calidad en Europa (Monde Selection y ITQT 2020).</t>
-  </si>
-  <si>
-    <t>· Cerveza ligera de bajo amargor, muy refrescante. · 30 días de elaboración (Doble que otras cervezas). · Producida con energía 100% renovable.</t>
-  </si>
-  <si>
-    <t>· Cerveza liviana. · Ritual único de lima, que le añade carácter, sabor y frescura.</t>
-  </si>
-  <si>
-    <t>· Cerveza del mercado chileno con más premios internacionales de calidad.  · 100% malta. · 4 variedades : Dorada, Trigo, Roja y Negra; ideales para acompañar
+    <t>Conocida como La Baltiloca.</t>
+  </si>
+  <si>
+    <t>Es la chela del pueblo y una de las más queridas por los chilenos.</t>
+  </si>
+  <si>
+    <t>3ra más vendida en Chile.</t>
+  </si>
+  <si>
+    <t>Premiada por su calidad en Europa (Monde Selection y ITQT 2020).</t>
+  </si>
+  <si>
+    <t>Fácil de beber, ligera, refrescante y siempre con un sabor superior.</t>
+  </si>
+  <si>
+    <t>Cerveza ligera de bajo amargor, muy refrescante.</t>
+  </si>
+  <si>
+    <t>30 días de elaboración (Doble que otras cervezas).</t>
+  </si>
+  <si>
+    <t>Producida con energía 100% renovable.</t>
+  </si>
+  <si>
+    <t>Cerveza liviana.</t>
+  </si>
+  <si>
+    <t>Ritual único de lima, que le añade carácter, sabor y frescura.</t>
+  </si>
+  <si>
+    <t>Cerveza del mercado chileno con más premios internacionales de calidad.</t>
+  </si>
+  <si>
+    <t>100% malta.</t>
+  </si>
+  <si>
+    <t>4 variedades : Dorada, Trigo, Roja y Negra; ideales para acompañar   las comidas.</t>
   </si>
   <si>
-    <t>· Goose IPA: Aroma cítrico con fuerte sabor a lúpulo. Seco pero suave. · Goose 312: Cuerpo suave y cremoso que logra una cerveza inmensamente refrescante.</t>
-  </si>
-  <si>
-    <t>· IPA de fácil tomabilidad, con un toque de sauco y miel. · Bohemian: Color Brillante y Aroma Maltoso. · Amber: Un suave sabor a caramelo.</t>
-  </si>
-  <si>
-    <t>· 100% malta y con 6 lúpulos. · Materias primas seleccionadas y mayor tiempo de maduración. · Principal auspiciador del Colo Colo. </t>
-  </si>
-  <si>
-    <t>· Elaborada con Lúpulo Saaz europeo patentado. · Variedad sin gluten, mismo sabor. · Premiada en 2020 como la mejor lager del mundo.</t>
+    <t>Goose IPA: Aroma cítrico con fuerte sabor a lúpulo. Seco pero suave.</t>
+  </si>
+  <si>
+    <t>Goose 312: Cuerpo suave y cremoso que logra una cerveza inmensamente refrescante.</t>
+  </si>
+  <si>
+    <t>IPA de fácil tomabilidad, con un toque de sauco y miel.</t>
+  </si>
+  <si>
+    <t>Bohemian: Color Brillante y Aroma Maltoso.</t>
+  </si>
+  <si>
+    <t>Amber: Un suave sabor a caramelo.</t>
+  </si>
+  <si>
+    <t>Cerveza premium de estilo lager, liviana y refrescante.</t>
+  </si>
+  <si>
+    <t>100% malta y con 6 lúpulos.</t>
+  </si>
+  <si>
+    <t>Materias primas seleccionadas y mayor tiempo de maduración . Principal auspiciador del Colo Colo</t>
+  </si>
+  <si>
+    <t>Cerveza dorada y equilibrada,  hecha con ingredientes naturales de campos argentinos.</t>
+  </si>
+  <si>
+    <t>Elaborada con Lúpulo Saaz europeo patentado.</t>
+  </si>
+  <si>
+    <t>Variedad sin gluten, mismo sabor.</t>
+  </si>
+  <si>
+    <t>Premiada en 2020 como la mejor lager del mundo.</t>
   </si>
 </sst>
 </file>
@@ -806,11 +845,58 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
@@ -827,56 +913,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -1238,8 +1277,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:M33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1293,92 +1332,96 @@
       <c r="M1" s="7"/>
     </row>
     <row r="2" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="20" t="s">
+      <c r="B2" s="35"/>
+      <c r="C2" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="22" t="s">
+      <c r="D2" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="24" t="s">
+      <c r="E2" s="30" t="s">
         <v>15</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="G2" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="G2" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="14" t="s">
+      <c r="H2" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
-      <c r="K2" s="15"/>
-      <c r="L2" s="15"/>
-      <c r="M2" s="14"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" s="17"/>
-      <c r="B3" s="19"/>
-      <c r="C3" s="21"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="15"/>
+    </row>
+    <row r="3" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+      <c r="A3" s="34"/>
+      <c r="B3" s="36"/>
+      <c r="C3" s="20"/>
       <c r="D3" s="23"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14"/>
-      <c r="L3" s="14"/>
-      <c r="M3" s="14"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="15"/>
+      <c r="L3" s="15"/>
+      <c r="M3" s="15"/>
     </row>
     <row r="4" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="28"/>
-      <c r="C4" s="21" t="s">
+      <c r="B4" s="19"/>
+      <c r="C4" s="20" t="s">
         <v>19</v>
       </c>
       <c r="D4" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="24" t="s">
+      <c r="E4" s="30" t="s">
         <v>21</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="G4" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="G4" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="H4" s="14" t="s">
+      <c r="H4" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="I4" s="14"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="14"/>
-      <c r="L4" s="14"/>
-      <c r="M4" s="14"/>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="27"/>
-      <c r="B5" s="28"/>
-      <c r="C5" s="21"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15"/>
+      <c r="K4" s="15"/>
+      <c r="L4" s="15"/>
+      <c r="M4" s="15"/>
+    </row>
+    <row r="5" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+      <c r="A5" s="18"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="20"/>
       <c r="D5" s="23"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="14"/>
-      <c r="L5" s="14"/>
-      <c r="M5" s="14"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
+      <c r="L5" s="15"/>
+      <c r="M5" s="15"/>
     </row>
     <row r="6" spans="1:13" ht="64" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
@@ -1424,13 +1467,13 @@
         <v>33</v>
       </c>
       <c r="F7" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="G7" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="H7" s="11" t="s">
         <v>35</v>
-      </c>
-      <c r="H7" s="11" t="s">
-        <v>36</v>
       </c>
       <c r="I7" s="7"/>
       <c r="J7" s="7"/>
@@ -1438,234 +1481,246 @@
       <c r="L7" s="7"/>
       <c r="M7" s="7"/>
     </row>
-    <row r="8" spans="1:13" ht="80" x14ac:dyDescent="0.2">
-      <c r="A8" s="26" t="s">
+    <row r="8" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+      <c r="A8" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" s="19"/>
+      <c r="C8" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="B8" s="28"/>
-      <c r="C8" s="21" t="s">
+      <c r="D8" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="D8" s="23" t="s">
+      <c r="E8" s="30" t="s">
         <v>39</v>
-      </c>
-      <c r="E8" s="24" t="s">
-        <v>40</v>
       </c>
       <c r="F8" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="G8" s="14" t="s">
+      <c r="G8" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="H8" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="15"/>
+      <c r="M8" s="15"/>
+    </row>
+    <row r="9" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+      <c r="A9" s="17"/>
+      <c r="B9" s="19"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="15"/>
+      <c r="M9" s="15"/>
+    </row>
+    <row r="10" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+      <c r="A10" s="18"/>
+      <c r="B10" s="19"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="15"/>
+      <c r="L10" s="15"/>
+      <c r="M10" s="15"/>
+    </row>
+    <row r="11" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" s="19"/>
+      <c r="C11" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="G11" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="H11" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="I11" s="15"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="15"/>
+      <c r="L11" s="15"/>
+      <c r="M11" s="15"/>
+    </row>
+    <row r="12" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+      <c r="A12" s="18"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="15"/>
+      <c r="J12" s="15"/>
+      <c r="K12" s="15"/>
+      <c r="L12" s="15"/>
+      <c r="M12" s="15"/>
+    </row>
+    <row r="13" spans="1:13" ht="48" x14ac:dyDescent="0.2">
+      <c r="A13" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" s="19"/>
+      <c r="C13" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="D13" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="G13" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="H13" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="I13" s="15"/>
+      <c r="J13" s="15"/>
+      <c r="K13" s="15"/>
+      <c r="L13" s="15"/>
+      <c r="M13" s="15"/>
+    </row>
+    <row r="14" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="A14" s="17"/>
+      <c r="B14" s="19"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
+      <c r="I14" s="15"/>
+      <c r="J14" s="15"/>
+      <c r="K14" s="15"/>
+      <c r="L14" s="15"/>
+      <c r="M14" s="15"/>
+    </row>
+    <row r="15" spans="1:13" ht="48" x14ac:dyDescent="0.2">
+      <c r="A15" s="18"/>
+      <c r="B15" s="19"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="15"/>
+      <c r="J15" s="15"/>
+      <c r="K15" s="15"/>
+      <c r="L15" s="15"/>
+      <c r="M15" s="15"/>
+    </row>
+    <row r="16" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+      <c r="A16" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="B16" s="19"/>
+      <c r="C16" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="D16" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="E16" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="G16" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="H16" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="H8" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="14"/>
-      <c r="L8" s="14"/>
-      <c r="M8" s="14"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A9" s="29"/>
-      <c r="B9" s="28"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="30"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="14"/>
-      <c r="L9" s="14"/>
-      <c r="M9" s="14"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A10" s="27"/>
-      <c r="B10" s="28"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="23"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="14"/>
-      <c r="L10" s="14"/>
-      <c r="M10" s="14"/>
-    </row>
-    <row r="11" spans="1:13" ht="48" x14ac:dyDescent="0.2">
-      <c r="A11" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="B11" s="28"/>
-      <c r="C11" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="D11" s="21" t="s">
-        <v>44</v>
-      </c>
-      <c r="E11" s="31" t="s">
-        <v>45</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="G11" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="H11" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="14"/>
-      <c r="L11" s="14"/>
-      <c r="M11" s="14"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A12" s="27"/>
-      <c r="B12" s="28"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="32"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="14"/>
-      <c r="L12" s="14"/>
-      <c r="M12" s="14"/>
-    </row>
-    <row r="13" spans="1:13" ht="96" x14ac:dyDescent="0.2">
-      <c r="A13" s="26" t="s">
-        <v>47</v>
-      </c>
-      <c r="B13" s="28"/>
-      <c r="C13" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="D13" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="E13" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="G13" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="H13" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="14"/>
-      <c r="L13" s="14"/>
-      <c r="M13" s="14"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A14" s="29"/>
-      <c r="B14" s="28"/>
-      <c r="C14" s="21"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
-      <c r="K14" s="14"/>
-      <c r="L14" s="14"/>
-      <c r="M14" s="14"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A15" s="27"/>
-      <c r="B15" s="28"/>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="33"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="14"/>
-      <c r="L15" s="14"/>
-      <c r="M15" s="14"/>
-    </row>
-    <row r="16" spans="1:13" ht="80" x14ac:dyDescent="0.2">
-      <c r="A16" s="26" t="s">
-        <v>53</v>
-      </c>
-      <c r="B16" s="28"/>
-      <c r="C16" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="D16" s="23" t="s">
-        <v>55</v>
-      </c>
-      <c r="E16" s="34" t="s">
-        <v>56</v>
-      </c>
-      <c r="F16" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="G16" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="H16" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="I16" s="14"/>
-      <c r="J16" s="14"/>
-      <c r="K16" s="14"/>
-      <c r="L16" s="14"/>
-      <c r="M16" s="14"/>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A17" s="27"/>
-      <c r="B17" s="28"/>
-      <c r="C17" s="21"/>
+      <c r="I16" s="15"/>
+      <c r="J16" s="15"/>
+      <c r="K16" s="15"/>
+      <c r="L16" s="15"/>
+      <c r="M16" s="15"/>
+    </row>
+    <row r="17" spans="1:13" ht="48" x14ac:dyDescent="0.2">
+      <c r="A17" s="18"/>
+      <c r="B17" s="19"/>
+      <c r="C17" s="20"/>
       <c r="D17" s="23"/>
-      <c r="E17" s="35"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="33"/>
-      <c r="I17" s="14"/>
-      <c r="J17" s="14"/>
-      <c r="K17" s="14"/>
-      <c r="L17" s="14"/>
-      <c r="M17" s="14"/>
+      <c r="E17" s="26"/>
+      <c r="F17" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="G17" s="15"/>
+      <c r="H17" s="27"/>
+      <c r="I17" s="15"/>
+      <c r="J17" s="15"/>
+      <c r="K17" s="15"/>
+      <c r="L17" s="15"/>
+      <c r="M17" s="15"/>
     </row>
     <row r="18" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A18" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B18" s="9"/>
       <c r="C18" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="E18" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="E18" s="12" t="s">
+      <c r="F18" s="7" t="s">
         <v>60</v>
-      </c>
-      <c r="F18" s="7" t="s">
-        <v>61</v>
       </c>
       <c r="G18" s="7" t="s">
         <v>28</v>
       </c>
       <c r="H18" s="12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I18" s="7"/>
       <c r="J18" s="7"/>
@@ -1673,87 +1728,91 @@
       <c r="L18" s="7"/>
       <c r="M18" s="7"/>
     </row>
-    <row r="19" spans="1:13" ht="64" x14ac:dyDescent="0.2">
-      <c r="A19" s="26" t="s">
+    <row r="19" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+      <c r="A19" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="B19" s="19"/>
+      <c r="C19" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="B19" s="28"/>
-      <c r="C19" s="21" t="s">
+      <c r="D19" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="D19" s="23" t="s">
+      <c r="E19" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="E19" s="34" t="s">
+      <c r="F19" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="G19" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="H19" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="F19" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="G19" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="H19" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="I19" s="14"/>
-      <c r="J19" s="14"/>
-      <c r="K19" s="14"/>
-      <c r="L19" s="14"/>
-      <c r="M19" s="14"/>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A20" s="29"/>
-      <c r="B20" s="28"/>
-      <c r="C20" s="21"/>
+      <c r="I19" s="15"/>
+      <c r="J19" s="15"/>
+      <c r="K19" s="15"/>
+      <c r="L19" s="15"/>
+      <c r="M19" s="15"/>
+    </row>
+    <row r="20" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+      <c r="A20" s="17"/>
+      <c r="B20" s="19"/>
+      <c r="C20" s="20"/>
       <c r="D20" s="23"/>
-      <c r="E20" s="36"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="14"/>
-      <c r="I20" s="14"/>
-      <c r="J20" s="14"/>
-      <c r="K20" s="14"/>
-      <c r="L20" s="14"/>
-      <c r="M20" s="14"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A21" s="27"/>
-      <c r="B21" s="28"/>
-      <c r="C21" s="21"/>
+      <c r="E20" s="25"/>
+      <c r="F20" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="G20" s="15"/>
+      <c r="H20" s="15"/>
+      <c r="I20" s="15"/>
+      <c r="J20" s="15"/>
+      <c r="K20" s="15"/>
+      <c r="L20" s="15"/>
+      <c r="M20" s="15"/>
+    </row>
+    <row r="21" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="A21" s="18"/>
+      <c r="B21" s="19"/>
+      <c r="C21" s="20"/>
       <c r="D21" s="23"/>
-      <c r="E21" s="35"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="14"/>
-      <c r="H21" s="14"/>
-      <c r="I21" s="14"/>
-      <c r="J21" s="14"/>
-      <c r="K21" s="14"/>
-      <c r="L21" s="14"/>
-      <c r="M21" s="14"/>
+      <c r="E21" s="26"/>
+      <c r="F21" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="G21" s="15"/>
+      <c r="H21" s="15"/>
+      <c r="I21" s="15"/>
+      <c r="J21" s="15"/>
+      <c r="K21" s="15"/>
+      <c r="L21" s="15"/>
+      <c r="M21" s="15"/>
     </row>
     <row r="22" spans="1:13" ht="64" x14ac:dyDescent="0.2">
       <c r="A22" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B22" s="9"/>
       <c r="C22" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="E22" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="E22" s="12" t="s">
+      <c r="F22" s="7" t="s">
         <v>71</v>
-      </c>
-      <c r="F22" s="7" t="s">
-        <v>72</v>
       </c>
       <c r="G22" s="7" t="s">
         <v>28</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I22" s="7"/>
       <c r="J22" s="7"/>
@@ -1763,26 +1822,26 @@
     </row>
     <row r="23" spans="1:13" ht="64" x14ac:dyDescent="0.2">
       <c r="A23" s="10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B23" s="9"/>
       <c r="C23" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="E23" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="E23" s="7" t="s">
+      <c r="F23" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="G23" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="F23" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="G23" s="7" t="s">
-        <v>78</v>
-      </c>
       <c r="H23" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I23" s="7"/>
       <c r="J23" s="7"/>
@@ -1792,26 +1851,26 @@
     </row>
     <row r="24" spans="1:13" ht="64" x14ac:dyDescent="0.2">
       <c r="A24" s="10" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B24" s="9"/>
       <c r="C24" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E24" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="F24" s="7" t="s">
         <v>80</v>
-      </c>
-      <c r="E24" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="F24" s="7" t="s">
-        <v>82</v>
       </c>
       <c r="G24" s="7" t="s">
         <v>28</v>
       </c>
       <c r="H24" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I24" s="7"/>
       <c r="J24" s="7"/>
@@ -1821,26 +1880,26 @@
     </row>
     <row r="25" spans="1:13" ht="64" x14ac:dyDescent="0.2">
       <c r="A25" s="10" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B25" s="9"/>
       <c r="C25" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E25" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="F25" s="7" t="s">
         <v>80</v>
-      </c>
-      <c r="E25" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="F25" s="7" t="s">
-        <v>82</v>
       </c>
       <c r="G25" s="7" t="s">
         <v>28</v>
       </c>
       <c r="H25" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I25" s="7"/>
       <c r="J25" s="7"/>
@@ -1850,23 +1909,23 @@
     </row>
     <row r="26" spans="1:13" ht="64" x14ac:dyDescent="0.2">
       <c r="A26" s="10" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B26" s="9"/>
       <c r="C26" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E26" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="F26" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="D26" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="E26" s="13" t="s">
-        <v>102</v>
-      </c>
-      <c r="F26" s="7" t="s">
-        <v>103</v>
-      </c>
       <c r="G26" s="7" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="H26" s="8" t="s">
         <v>17</v>
@@ -1877,152 +1936,158 @@
       <c r="L26" s="7"/>
       <c r="M26" s="7"/>
     </row>
-    <row r="27" spans="1:13" ht="80" x14ac:dyDescent="0.2">
-      <c r="A27" s="26" t="s">
+    <row r="27" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="A27" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="B27" s="19"/>
+      <c r="C27" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="D27" s="23" t="s">
         <v>83</v>
       </c>
-      <c r="B27" s="28"/>
-      <c r="C27" s="21" t="s">
+      <c r="E27" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="D27" s="23" t="s">
+      <c r="F27" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="G27" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="H27" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="I27" s="15"/>
+      <c r="J27" s="15"/>
+      <c r="K27" s="15"/>
+      <c r="L27" s="15"/>
+      <c r="M27" s="15"/>
+    </row>
+    <row r="28" spans="1:13" ht="48" x14ac:dyDescent="0.2">
+      <c r="A28" s="18"/>
+      <c r="B28" s="19"/>
+      <c r="C28" s="20"/>
+      <c r="D28" s="23"/>
+      <c r="E28" s="26"/>
+      <c r="F28" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="G28" s="15"/>
+      <c r="H28" s="22"/>
+      <c r="I28" s="15"/>
+      <c r="J28" s="15"/>
+      <c r="K28" s="15"/>
+      <c r="L28" s="15"/>
+      <c r="M28" s="15"/>
+    </row>
+    <row r="29" spans="1:13" ht="64" x14ac:dyDescent="0.2">
+      <c r="A29" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="E27" s="34" t="s">
+      <c r="B29" s="9"/>
+      <c r="C29" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="F27" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="G27" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="H27" s="37" t="s">
-        <v>17</v>
-      </c>
-      <c r="I27" s="14"/>
-      <c r="J27" s="14"/>
-      <c r="K27" s="14"/>
-      <c r="L27" s="14"/>
-      <c r="M27" s="14"/>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A28" s="29"/>
-      <c r="B28" s="28"/>
-      <c r="C28" s="21"/>
-      <c r="D28" s="23"/>
-      <c r="E28" s="36"/>
-      <c r="F28" s="7"/>
-      <c r="G28" s="14"/>
-      <c r="H28" s="37"/>
-      <c r="I28" s="14"/>
-      <c r="J28" s="14"/>
-      <c r="K28" s="14"/>
-      <c r="L28" s="14"/>
-      <c r="M28" s="14"/>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A29" s="27"/>
-      <c r="B29" s="28"/>
-      <c r="C29" s="21"/>
-      <c r="D29" s="23"/>
-      <c r="E29" s="35"/>
-      <c r="F29" s="7"/>
-      <c r="G29" s="14"/>
-      <c r="H29" s="38"/>
-      <c r="I29" s="14"/>
-      <c r="J29" s="14"/>
-      <c r="K29" s="14"/>
-      <c r="L29" s="14"/>
-      <c r="M29" s="14"/>
-    </row>
-    <row r="30" spans="1:13" ht="64" x14ac:dyDescent="0.2">
-      <c r="A30" s="10" t="s">
+      <c r="D29" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B30" s="9"/>
-      <c r="C30" s="1" t="s">
+      <c r="E29" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="D30" s="1" t="s">
+      <c r="F29" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="G29" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="H29" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="I29" s="7"/>
+      <c r="J29" s="7"/>
+      <c r="K29" s="7"/>
+      <c r="L29" s="7"/>
+      <c r="M29" s="7"/>
+    </row>
+    <row r="30" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+      <c r="A30" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="E30" s="12" t="s">
+      <c r="B30" s="19"/>
+      <c r="C30" s="20" t="s">
         <v>90</v>
       </c>
+      <c r="D30" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="E30" s="14" t="s">
+        <v>92</v>
+      </c>
       <c r="F30" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="G30" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="H30" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="I30" s="7"/>
-      <c r="J30" s="7"/>
-      <c r="K30" s="7"/>
-      <c r="L30" s="7"/>
-      <c r="M30" s="7"/>
-    </row>
-    <row r="31" spans="1:13" ht="80" x14ac:dyDescent="0.2">
-      <c r="A31" s="26" t="s">
-        <v>92</v>
-      </c>
-      <c r="B31" s="28"/>
-      <c r="C31" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="G30" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="D31" s="21" t="s">
-        <v>94</v>
-      </c>
-      <c r="E31" s="15" t="s">
-        <v>95</v>
-      </c>
+      <c r="H30" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="I30" s="15"/>
+      <c r="J30" s="15"/>
+      <c r="K30" s="15"/>
+      <c r="L30" s="15"/>
+      <c r="M30" s="15"/>
+    </row>
+    <row r="31" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="A31" s="17"/>
+      <c r="B31" s="19"/>
+      <c r="C31" s="20"/>
+      <c r="D31" s="20"/>
+      <c r="E31" s="15"/>
       <c r="F31" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="G31" s="14" t="s">
-        <v>96</v>
-      </c>
-      <c r="H31" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="I31" s="14"/>
-      <c r="J31" s="14"/>
-      <c r="K31" s="14"/>
-      <c r="L31" s="14"/>
-      <c r="M31" s="14"/>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A32" s="29"/>
-      <c r="B32" s="28"/>
-      <c r="C32" s="21"/>
-      <c r="D32" s="21"/>
-      <c r="E32" s="14"/>
-      <c r="F32" s="7"/>
-      <c r="G32" s="14"/>
-      <c r="H32" s="14"/>
-      <c r="I32" s="14"/>
-      <c r="J32" s="14"/>
-      <c r="K32" s="14"/>
-      <c r="L32" s="14"/>
-      <c r="M32" s="14"/>
+        <v>124</v>
+      </c>
+      <c r="G31" s="15"/>
+      <c r="H31" s="15"/>
+      <c r="I31" s="15"/>
+      <c r="J31" s="15"/>
+      <c r="K31" s="15"/>
+      <c r="L31" s="15"/>
+      <c r="M31" s="15"/>
+    </row>
+    <row r="32" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+      <c r="A32" s="18"/>
+      <c r="B32" s="19"/>
+      <c r="C32" s="20"/>
+      <c r="D32" s="20"/>
+      <c r="E32" s="15"/>
+      <c r="F32" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="G32" s="15"/>
+      <c r="H32" s="15"/>
+      <c r="I32" s="15"/>
+      <c r="J32" s="15"/>
+      <c r="K32" s="15"/>
+      <c r="L32" s="15"/>
+      <c r="M32" s="15"/>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A33" s="27"/>
-      <c r="B33" s="28"/>
-      <c r="C33" s="21"/>
-      <c r="D33" s="21"/>
-      <c r="E33" s="14"/>
+      <c r="A33" s="7"/>
+      <c r="B33" s="7"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
       <c r="F33" s="7"/>
-      <c r="G33" s="14"/>
-      <c r="H33" s="14"/>
-      <c r="I33" s="14"/>
-      <c r="J33" s="14"/>
-      <c r="K33" s="14"/>
-      <c r="L33" s="14"/>
-      <c r="M33" s="14"/>
+      <c r="G33" s="7"/>
+      <c r="H33" s="7"/>
+      <c r="I33" s="7"/>
+      <c r="J33" s="7"/>
+      <c r="K33" s="7"/>
+      <c r="L33" s="7"/>
+      <c r="M33" s="7"/>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" s="7"/>
@@ -2041,30 +2106,78 @@
     </row>
   </sheetData>
   <mergeCells count="108">
-    <mergeCell ref="H31:H33"/>
-    <mergeCell ref="I31:I33"/>
-    <mergeCell ref="J31:J33"/>
-    <mergeCell ref="K31:K33"/>
-    <mergeCell ref="L31:L33"/>
-    <mergeCell ref="M31:M33"/>
-    <mergeCell ref="A31:A33"/>
-    <mergeCell ref="B31:B33"/>
-    <mergeCell ref="C31:C33"/>
-    <mergeCell ref="D31:D33"/>
-    <mergeCell ref="E31:E33"/>
-    <mergeCell ref="G31:G33"/>
-    <mergeCell ref="H27:H29"/>
-    <mergeCell ref="I27:I29"/>
-    <mergeCell ref="J27:J29"/>
-    <mergeCell ref="K27:K29"/>
-    <mergeCell ref="L27:L29"/>
-    <mergeCell ref="M27:M29"/>
-    <mergeCell ref="A27:A29"/>
-    <mergeCell ref="B27:B29"/>
-    <mergeCell ref="C27:C29"/>
-    <mergeCell ref="D27:D29"/>
-    <mergeCell ref="E27:E29"/>
-    <mergeCell ref="G27:G29"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="K2:K3"/>
+    <mergeCell ref="L2:L3"/>
+    <mergeCell ref="M2:M3"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="I4:I5"/>
+    <mergeCell ref="J4:J5"/>
+    <mergeCell ref="K4:K5"/>
+    <mergeCell ref="L4:L5"/>
+    <mergeCell ref="M4:M5"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="H8:H10"/>
+    <mergeCell ref="I8:I10"/>
+    <mergeCell ref="J8:J10"/>
+    <mergeCell ref="K8:K10"/>
+    <mergeCell ref="L8:L10"/>
+    <mergeCell ref="M8:M10"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="E8:E10"/>
+    <mergeCell ref="G8:G10"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="J11:J12"/>
+    <mergeCell ref="K11:K12"/>
+    <mergeCell ref="L11:L12"/>
+    <mergeCell ref="M11:M12"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="H13:H15"/>
+    <mergeCell ref="I13:I15"/>
+    <mergeCell ref="J13:J15"/>
+    <mergeCell ref="K13:K15"/>
+    <mergeCell ref="L13:L15"/>
+    <mergeCell ref="M13:M15"/>
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="C13:C15"/>
+    <mergeCell ref="D13:D15"/>
+    <mergeCell ref="E13:E15"/>
+    <mergeCell ref="G13:G15"/>
+    <mergeCell ref="H16:H17"/>
+    <mergeCell ref="I16:I17"/>
+    <mergeCell ref="J16:J17"/>
+    <mergeCell ref="K16:K17"/>
+    <mergeCell ref="L16:L17"/>
+    <mergeCell ref="M16:M17"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="G16:G17"/>
     <mergeCell ref="H19:H21"/>
     <mergeCell ref="I19:I21"/>
     <mergeCell ref="J19:J21"/>
@@ -2077,116 +2190,68 @@
     <mergeCell ref="D19:D21"/>
     <mergeCell ref="E19:E21"/>
     <mergeCell ref="G19:G21"/>
-    <mergeCell ref="H16:H17"/>
-    <mergeCell ref="I16:I17"/>
-    <mergeCell ref="J16:J17"/>
-    <mergeCell ref="K16:K17"/>
-    <mergeCell ref="L16:L17"/>
-    <mergeCell ref="M16:M17"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="G16:G17"/>
-    <mergeCell ref="H13:H15"/>
-    <mergeCell ref="I13:I15"/>
-    <mergeCell ref="J13:J15"/>
-    <mergeCell ref="K13:K15"/>
-    <mergeCell ref="L13:L15"/>
-    <mergeCell ref="M13:M15"/>
-    <mergeCell ref="A13:A15"/>
-    <mergeCell ref="B13:B15"/>
-    <mergeCell ref="C13:C15"/>
-    <mergeCell ref="D13:D15"/>
-    <mergeCell ref="E13:E15"/>
-    <mergeCell ref="G13:G15"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="J11:J12"/>
-    <mergeCell ref="K11:K12"/>
-    <mergeCell ref="L11:L12"/>
-    <mergeCell ref="M11:M12"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="H8:H10"/>
-    <mergeCell ref="I8:I10"/>
-    <mergeCell ref="J8:J10"/>
-    <mergeCell ref="K8:K10"/>
-    <mergeCell ref="L8:L10"/>
-    <mergeCell ref="M8:M10"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="D8:D10"/>
-    <mergeCell ref="E8:E10"/>
-    <mergeCell ref="G8:G10"/>
-    <mergeCell ref="H4:H5"/>
-    <mergeCell ref="I4:I5"/>
-    <mergeCell ref="J4:J5"/>
-    <mergeCell ref="K4:K5"/>
-    <mergeCell ref="L4:L5"/>
-    <mergeCell ref="M4:M5"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="G4:G5"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="J2:J3"/>
-    <mergeCell ref="K2:K3"/>
-    <mergeCell ref="L2:L3"/>
-    <mergeCell ref="M2:M3"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="G27:G28"/>
+    <mergeCell ref="H27:H28"/>
+    <mergeCell ref="I27:I28"/>
+    <mergeCell ref="J27:J28"/>
+    <mergeCell ref="K27:K28"/>
+    <mergeCell ref="L27:L28"/>
+    <mergeCell ref="M27:M28"/>
+    <mergeCell ref="A30:A32"/>
+    <mergeCell ref="B30:B32"/>
+    <mergeCell ref="C30:C32"/>
+    <mergeCell ref="D30:D32"/>
+    <mergeCell ref="E30:E32"/>
+    <mergeCell ref="G30:G32"/>
+    <mergeCell ref="H30:H32"/>
+    <mergeCell ref="I30:I32"/>
+    <mergeCell ref="J30:J32"/>
+    <mergeCell ref="K30:K32"/>
+    <mergeCell ref="L30:L32"/>
+    <mergeCell ref="M30:M32"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="https://res.cloudinary.com/dkktirn06/image/upload/v1662093417/BANNERS KOA KOE/baltica-SKUS-banners-KOA-KOE-catalogo-400x400_qcu6m8.png" xr:uid="{2C61CC60-D728-BC42-9684-CE9DB4D8EEA9}"/>
-    <hyperlink ref="D2" r:id="rId2" display="https://res.cloudinary.com/dkktirn06/image/upload/v1662093427/BANNERS KOA KOE/baltica-banners-KOA-KOE-catalogo-1920x400_y6nxcq.png" xr:uid="{2EE5CD3F-4426-AF45-A25F-D1AE9CDB961B}"/>
-    <hyperlink ref="C4" r:id="rId3" display="https://res.cloudinary.com/dkktirn06/image/upload/v1662526228/BANNERS KOA KOE/Becker-SKUS-banners-KOA-KOE-catalogo-400x400_a8lqjo.png" xr:uid="{935522B9-A553-7D40-95C9-30D86875C3AE}"/>
-    <hyperlink ref="D4" r:id="rId4" display="https://res.cloudinary.com/dkktirn06/image/upload/v1662130736/BANNERS KOA KOE/beckrer-banners-KOA-KOE-catalogo-1920x400_h9vizn.png" xr:uid="{DB012BC4-B5C1-9444-91C3-97D5ADBB93E9}"/>
-    <hyperlink ref="C6" r:id="rId5" display="https://res.cloudinary.com/dkktirn06/image/upload/v1663854946/BANNERS KOA KOE/becks-SKUS-banners-KOA-KOE-catalogo-400x400_orrppj.png" xr:uid="{EC905F6F-0C1D-1A41-A0A7-CA770E3FDA8D}"/>
-    <hyperlink ref="D6" r:id="rId6" display="https://res.cloudinary.com/dkktirn06/image/upload/v1662484301/BANNERS KOA KOE/becks-banners-KOA-KOE-catalogo-1920x400_fhuocn.png" xr:uid="{3D4D1AF1-E74C-314E-9E7F-A8F044DC0062}"/>
-    <hyperlink ref="C7" r:id="rId7" display="https://res.cloudinary.com/dkktirn06/image/upload/v1662488171/BANNERS KOA KOE/budlight-SKUS-banners-KOA-KOE-catalogo-400x400_zocurr.png" xr:uid="{F9153934-9904-F543-808E-B28EE736212B}"/>
-    <hyperlink ref="D7" r:id="rId8" display="https://res.cloudinary.com/dkktirn06/image/upload/v1662487671/BANNERS KOA KOE/budlight-banners-KOA-KOE-catalogo-1920x400_ireh1n.png" xr:uid="{F4366488-B1AB-A649-BE7F-E673FFAE5399}"/>
-    <hyperlink ref="C8" r:id="rId9" display="https://res.cloudinary.com/dkktirn06/image/upload/v1662493678/BANNERS KOA KOE/Budweiser-SKUS-banners-KOA-KOE-catalogo-400x400_dfffen.png" xr:uid="{492A0019-6FC6-AB40-BEA4-35A4DB7C023C}"/>
-    <hyperlink ref="D8" r:id="rId10" display="https://res.cloudinary.com/dkktirn06/image/upload/v1662493781/BANNERS KOA KOE/Budweiser-banners-KOA-KOE-catalogo-1920x400_gm3w3a.png" xr:uid="{67C2CD04-C4C3-364E-88D4-E54E2032F979}"/>
-    <hyperlink ref="C11" r:id="rId11" display="https://res.cloudinary.com/dkktirn06/image/upload/v1663855485/BANNERS KOA KOE/CORONA-SKUS-banners-KOA-KOE-catalogo-400x400_uewskk.png" xr:uid="{7F33F92D-8EE3-EB46-9E57-5B3DB31F9266}"/>
-    <hyperlink ref="D11" r:id="rId12" display="https://res.cloudinary.com/dkktirn06/image/upload/v1662056903/BANNERS KOA KOE/back_corona_KOA_TEST_btfhgu.png" xr:uid="{0B46C2F9-606A-C545-89B5-CD66C220D635}"/>
-    <hyperlink ref="C13" r:id="rId13" display="https://res.cloudinary.com/dkktirn06/image/upload/v1662496012/BANNERS KOA KOE/Cusquena-SKUS-banners-KOA-KOE-catalogo-400x400_v9anoi.png" xr:uid="{F489A020-B14E-3E46-B221-A6B8C5D8914A}"/>
-    <hyperlink ref="D13" r:id="rId14" display="https://res.cloudinary.com/dkktirn06/image/upload/v1662495503/BANNERS KOA KOE/Cusquena-banners-KOA-KOE-catalogo-1920x400_sgcxpu.png" xr:uid="{B146F557-DEE3-4444-9175-6D8F732DA6B9}"/>
-    <hyperlink ref="C16" r:id="rId15" display="https://res.cloudinary.com/dkktirn06/image/upload/v1663855647/BANNERS KOA KOE/Goose-Island-SKUS-banners-KOA-KOE-catalogo-400x400_kfuli4.png" xr:uid="{BE5F4015-30DE-434F-8A57-45A4B71F75B2}"/>
-    <hyperlink ref="D16" r:id="rId16" display="https://res.cloudinary.com/dkktirn06/image/upload/v1662498416/BANNERS KOA KOE/Goose-Island-banners-KOA-KOE-catalogo-1920x400_u9x5wj.png" xr:uid="{14AB3ABD-2D56-5B4B-ABD8-231EDCB90737}"/>
-    <hyperlink ref="C18" r:id="rId17" display="https://res.cloudinary.com/dkktirn06/image/upload/v1662515629/BANNERS KOA KOE/Hoegaarden-SKUS-banners-KOA-KOE-catalogo-400x400_zksmrj.png" xr:uid="{CA4FB07A-FF5B-1A49-84EF-0A13A7F90016}"/>
-    <hyperlink ref="D18" r:id="rId18" display="https://res.cloudinary.com/dkktirn06/image/upload/v1662515411/BANNERS KOA KOE/Hoegaarden-banners-KOA-KOE-catalogo-1920x400_e5pww4.png" xr:uid="{34D00E6E-4524-2C43-B8C4-9428FDA8A903}"/>
-    <hyperlink ref="C19" r:id="rId19" display="https://res.cloudinary.com/dkktirn06/image/upload/v1662516283/BANNERS KOA KOE/Km247-SKUS-banners-KOA-KOE-catalogo-400x400_h9tzs0.png" xr:uid="{931A340E-7B99-2A45-8AF9-CD400208629B}"/>
-    <hyperlink ref="D19" r:id="rId20" display="https://res.cloudinary.com/dkktirn06/image/upload/v1662516100/BANNERS KOA KOE/Km247-banners-KOA-KOE-catalogo-1920x400_j6hlu0.png" xr:uid="{752BDA6A-2CB7-FA41-B22D-A1E3038FE67C}"/>
-    <hyperlink ref="C22" r:id="rId21" display="https://res.cloudinary.com/dkktirn06/image/upload/v1662529232/BANNERS KOA KOE/Leffe-SKUS-banners-KOA-KOE-catalogo-400x400_lasidb.png" xr:uid="{988AD4FA-4E72-3247-B769-D64AB0A7E244}"/>
-    <hyperlink ref="D22" r:id="rId22" display="https://res.cloudinary.com/dkktirn06/image/upload/v1662528989/BANNERS KOA KOE/Leffe-KOA-KOE-catalogo-1920x400_rj8po5.png" xr:uid="{85EFF18C-65C0-C649-A0EF-4B89436486BA}"/>
-    <hyperlink ref="C23" r:id="rId23" display="https://res.cloudinary.com/dkktirn06/image/upload/v1662502925/BANNERS KOA KOE/Michelob-SKUS-banners-KOA-KOE-catalogo-400x400_rp3kkr.png" xr:uid="{0A36AB54-903E-1142-B409-7BFA13BD16BC}"/>
-    <hyperlink ref="D23" r:id="rId24" display="https://res.cloudinary.com/dkktirn06/image/upload/v1662502847/BANNERS KOA KOE/Michelob-banners-KOA-KOE-catalogo-1920x400_mbzruh.png" xr:uid="{9ADB558B-C501-B548-99CC-4BABBEBA23D1}"/>
-    <hyperlink ref="C24" r:id="rId25" display="https://res.cloudinary.com/dkktirn06/image/upload/v1663855984/BANNERS KOA KOE/Modelo-SKUS-banners-KOA-KOE-catalogo-400x400_k6mrl9.png" xr:uid="{C0C7DB19-32D2-274A-983E-4BF80DC46EAE}"/>
-    <hyperlink ref="D24" r:id="rId26" display="https://res.cloudinary.com/dkktirn06/image/upload/v1662522482/BANNERS KOA KOE/Modelo-KOA-KOE-catalogo-1920x400_qlscvd.png" xr:uid="{A8A0A4F9-17A0-E443-9ED6-946EDA8ECBA5}"/>
-    <hyperlink ref="C25" r:id="rId27" display="https://res.cloudinary.com/dkktirn06/image/upload/v1663855984/BANNERS KOA KOE/Modelo-SKUS-banners-KOA-KOE-catalogo-400x400_k6mrl9.png" xr:uid="{74C58616-915A-6840-9CF5-0C9CFED4B3E3}"/>
-    <hyperlink ref="D25" r:id="rId28" display="https://res.cloudinary.com/dkktirn06/image/upload/v1662522482/BANNERS KOA KOE/Modelo-KOA-KOE-catalogo-1920x400_qlscvd.png" xr:uid="{4A2E37C6-C633-7141-B943-322E64D3EA63}"/>
-    <hyperlink ref="C26" r:id="rId29" display="https://res.cloudinary.com/dkktirn06/image/upload/v1668873193/BANNERS KOA KOE/Malta-del-sur-SKUS-banners-KOA-KOE-catalogo-400x400_lvcpwp.png" xr:uid="{0D2E2D0A-C9E9-2345-893A-8EF6504300A6}"/>
-    <hyperlink ref="D26" r:id="rId30" display="https://res.cloudinary.com/dkktirn06/image/upload/v1668870138/BANNERS KOA KOE/malta_del_sur_KOA_KOE_catalogo_1920x400_de1noj.png" xr:uid="{96D4C304-FE8E-224E-8D0B-C157CAA38F4E}"/>
-    <hyperlink ref="C27" r:id="rId31" display="https://res.cloudinary.com/dkktirn06/image/upload/v1662524670/BANNERS KOA KOE/Pilsen-del-sur-KOA-KOE-catalogo-1920x400_svnnyg.png" xr:uid="{890AA228-13C7-2B4C-80A3-707252B3D540}"/>
-    <hyperlink ref="D27" r:id="rId32" display="https://res.cloudinary.com/dkktirn06/image/upload/v1662524068/BANNERS KOA KOE/Pilsen-KOA-KOE-catalogo-1920x400_xtmpvj.png" xr:uid="{69EA45B2-77B3-474E-A61F-571800BE68EB}"/>
-    <hyperlink ref="C30" r:id="rId33" display="https://res.cloudinary.com/dkktirn06/image/upload/v1662526158/BANNERS KOA KOE/Quilmes-SKUS-banners-KOA-KOE-catalogo-400x400_szyuaz.png" xr:uid="{A4AAB958-B039-1C41-B075-BB8D758E8801}"/>
-    <hyperlink ref="D30" r:id="rId34" display="https://res.cloudinary.com/dkktirn06/image/upload/v1662526118/BANNERS KOA KOE/Quilmes-KOA-KOE-catalogo-1920x400_fameyv.png" xr:uid="{E708942C-01D2-8945-A84A-570EAA138214}"/>
-    <hyperlink ref="C31" r:id="rId35" display="https://res.cloudinary.com/dkktirn06/image/upload/v1663856219/BANNERS KOA KOE/Stella-Artois-SKUS-banners-KOA-KOE-catalogo-400x400_t4y3va.png" xr:uid="{20BD3D4F-542F-6546-B2B1-EC830D34087C}"/>
-    <hyperlink ref="D31" r:id="rId36" display="https://res.cloudinary.com/dkktirn06/image/upload/v1662525249/BANNERS KOA KOE/Stella-Artois-KOA-KOE-catalogo-1920x400_zlqada.png" xr:uid="{93C7F7A2-8E6D-6647-BF9F-EE17AA24F23E}"/>
+    <hyperlink ref="C2" r:id="rId1" display="https://res.cloudinary.com/dkktirn06/image/upload/v1662093417/BANNERS KOA KOE/baltica-SKUS-banners-KOA-KOE-catalogo-400x400_qcu6m8.png" xr:uid="{2AB83645-1015-5749-B8C8-BF3CCB1543B8}"/>
+    <hyperlink ref="D2" r:id="rId2" display="https://res.cloudinary.com/dkktirn06/image/upload/v1662093427/BANNERS KOA KOE/baltica-banners-KOA-KOE-catalogo-1920x400_y6nxcq.png" xr:uid="{C3682B8D-7333-AB47-B02C-87F78E1C28BB}"/>
+    <hyperlink ref="C4" r:id="rId3" display="https://res.cloudinary.com/dkktirn06/image/upload/v1662526228/BANNERS KOA KOE/Becker-SKUS-banners-KOA-KOE-catalogo-400x400_a8lqjo.png" xr:uid="{7EFD587B-017D-A940-B707-7962D37FEA5A}"/>
+    <hyperlink ref="D4" r:id="rId4" display="https://res.cloudinary.com/dkktirn06/image/upload/v1662130736/BANNERS KOA KOE/beckrer-banners-KOA-KOE-catalogo-1920x400_h9vizn.png" xr:uid="{987498D4-4CD9-BB43-A07A-8A8C0094DA19}"/>
+    <hyperlink ref="C6" r:id="rId5" display="https://res.cloudinary.com/dkktirn06/image/upload/v1663854946/BANNERS KOA KOE/becks-SKUS-banners-KOA-KOE-catalogo-400x400_orrppj.png" xr:uid="{6E1F2BE5-21F3-514A-908F-28C7AD0228E2}"/>
+    <hyperlink ref="D6" r:id="rId6" display="https://res.cloudinary.com/dkktirn06/image/upload/v1662484301/BANNERS KOA KOE/becks-banners-KOA-KOE-catalogo-1920x400_fhuocn.png" xr:uid="{40F05037-0A1F-D847-A19B-E3950981E053}"/>
+    <hyperlink ref="C7" r:id="rId7" display="https://res.cloudinary.com/dkktirn06/image/upload/v1662488171/BANNERS KOA KOE/budlight-SKUS-banners-KOA-KOE-catalogo-400x400_zocurr.png" xr:uid="{5A84C5A2-CFC3-4C4A-8773-8ABB22A45EB7}"/>
+    <hyperlink ref="D7" r:id="rId8" display="https://res.cloudinary.com/dkktirn06/image/upload/v1662487671/BANNERS KOA KOE/budlight-banners-KOA-KOE-catalogo-1920x400_ireh1n.png" xr:uid="{45978426-ED7B-5841-9970-2256EF49AED7}"/>
+    <hyperlink ref="C8" r:id="rId9" display="https://res.cloudinary.com/dkktirn06/image/upload/v1662493678/BANNERS KOA KOE/Budweiser-SKUS-banners-KOA-KOE-catalogo-400x400_dfffen.png" xr:uid="{549A97F8-F913-1C40-9EB4-3665BF099144}"/>
+    <hyperlink ref="D8" r:id="rId10" display="https://res.cloudinary.com/dkktirn06/image/upload/v1662493781/BANNERS KOA KOE/Budweiser-banners-KOA-KOE-catalogo-1920x400_gm3w3a.png" xr:uid="{4491295A-7B09-B242-86D3-AD543BB03612}"/>
+    <hyperlink ref="C11" r:id="rId11" display="https://res.cloudinary.com/dkktirn06/image/upload/v1663855485/BANNERS KOA KOE/CORONA-SKUS-banners-KOA-KOE-catalogo-400x400_uewskk.png" xr:uid="{B97713D0-8842-BB40-9390-20718081E391}"/>
+    <hyperlink ref="D11" r:id="rId12" display="https://res.cloudinary.com/dkktirn06/image/upload/v1662056903/BANNERS KOA KOE/back_corona_KOA_TEST_btfhgu.png" xr:uid="{42610617-CF7F-CC4E-AC71-31416DB73590}"/>
+    <hyperlink ref="C13" r:id="rId13" display="https://res.cloudinary.com/dkktirn06/image/upload/v1662496012/BANNERS KOA KOE/Cusquena-SKUS-banners-KOA-KOE-catalogo-400x400_v9anoi.png" xr:uid="{25598A14-B902-784B-86D6-0B13D502DEB3}"/>
+    <hyperlink ref="D13" r:id="rId14" display="https://res.cloudinary.com/dkktirn06/image/upload/v1662495503/BANNERS KOA KOE/Cusquena-banners-KOA-KOE-catalogo-1920x400_sgcxpu.png" xr:uid="{BA6151FD-330F-294E-8130-2FE2BE9D12D8}"/>
+    <hyperlink ref="C16" r:id="rId15" display="https://res.cloudinary.com/dkktirn06/image/upload/v1663855647/BANNERS KOA KOE/Goose-Island-SKUS-banners-KOA-KOE-catalogo-400x400_kfuli4.png" xr:uid="{CCFF7121-2615-BD4A-A769-A71EAF2BD920}"/>
+    <hyperlink ref="D16" r:id="rId16" display="https://res.cloudinary.com/dkktirn06/image/upload/v1662498416/BANNERS KOA KOE/Goose-Island-banners-KOA-KOE-catalogo-1920x400_u9x5wj.png" xr:uid="{1F00651E-C2CC-0F4A-BA0B-6AAB2FE9C986}"/>
+    <hyperlink ref="C18" r:id="rId17" display="https://res.cloudinary.com/dkktirn06/image/upload/v1662515629/BANNERS KOA KOE/Hoegaarden-SKUS-banners-KOA-KOE-catalogo-400x400_zksmrj.png" xr:uid="{DA2D557C-7CE9-C647-A2F3-110AB1C72562}"/>
+    <hyperlink ref="D18" r:id="rId18" display="https://res.cloudinary.com/dkktirn06/image/upload/v1662515411/BANNERS KOA KOE/Hoegaarden-banners-KOA-KOE-catalogo-1920x400_e5pww4.png" xr:uid="{154B2FC7-5305-6645-82BF-F9A906FEDA70}"/>
+    <hyperlink ref="C19" r:id="rId19" display="https://res.cloudinary.com/dkktirn06/image/upload/v1662516283/BANNERS KOA KOE/Km247-SKUS-banners-KOA-KOE-catalogo-400x400_h9tzs0.png" xr:uid="{5A73B9FE-F49D-F54A-9DA8-6FFAE9AB67F3}"/>
+    <hyperlink ref="D19" r:id="rId20" display="https://res.cloudinary.com/dkktirn06/image/upload/v1662516100/BANNERS KOA KOE/Km247-banners-KOA-KOE-catalogo-1920x400_j6hlu0.png" xr:uid="{E3E69A59-FDC0-F646-AD4E-1C8416C9E35D}"/>
+    <hyperlink ref="C22" r:id="rId21" display="https://res.cloudinary.com/dkktirn06/image/upload/v1662529232/BANNERS KOA KOE/Leffe-SKUS-banners-KOA-KOE-catalogo-400x400_lasidb.png" xr:uid="{993CF6C5-1E3C-A948-93B7-46136D91C93F}"/>
+    <hyperlink ref="D22" r:id="rId22" display="https://res.cloudinary.com/dkktirn06/image/upload/v1662528989/BANNERS KOA KOE/Leffe-KOA-KOE-catalogo-1920x400_rj8po5.png" xr:uid="{62936589-C489-9144-9092-E9203C7D99C4}"/>
+    <hyperlink ref="C23" r:id="rId23" display="https://res.cloudinary.com/dkktirn06/image/upload/v1662502925/BANNERS KOA KOE/Michelob-SKUS-banners-KOA-KOE-catalogo-400x400_rp3kkr.png" xr:uid="{C72DA7B7-403F-7340-9C04-FFF058E90195}"/>
+    <hyperlink ref="D23" r:id="rId24" display="https://res.cloudinary.com/dkktirn06/image/upload/v1662502847/BANNERS KOA KOE/Michelob-banners-KOA-KOE-catalogo-1920x400_mbzruh.png" xr:uid="{A6F84A45-6796-F342-84D3-18D089ED7AD6}"/>
+    <hyperlink ref="C24" r:id="rId25" display="https://res.cloudinary.com/dkktirn06/image/upload/v1663855984/BANNERS KOA KOE/Modelo-SKUS-banners-KOA-KOE-catalogo-400x400_k6mrl9.png" xr:uid="{E804BECE-9655-EB45-94ED-003A1041F83A}"/>
+    <hyperlink ref="D24" r:id="rId26" display="https://res.cloudinary.com/dkktirn06/image/upload/v1662522482/BANNERS KOA KOE/Modelo-KOA-KOE-catalogo-1920x400_qlscvd.png" xr:uid="{E5DD7AF9-B218-4A4F-B280-1377806136A9}"/>
+    <hyperlink ref="C25" r:id="rId27" display="https://res.cloudinary.com/dkktirn06/image/upload/v1663855984/BANNERS KOA KOE/Modelo-SKUS-banners-KOA-KOE-catalogo-400x400_k6mrl9.png" xr:uid="{F6C3BD39-D5D1-694C-87DF-84A4AC5D9D65}"/>
+    <hyperlink ref="D25" r:id="rId28" display="https://res.cloudinary.com/dkktirn06/image/upload/v1662522482/BANNERS KOA KOE/Modelo-KOA-KOE-catalogo-1920x400_qlscvd.png" xr:uid="{847A5C95-9BE7-7749-B114-D042207BB29A}"/>
+    <hyperlink ref="C26" r:id="rId29" display="https://res.cloudinary.com/dkktirn06/image/upload/v1668873193/BANNERS KOA KOE/Malta-del-sur-SKUS-banners-KOA-KOE-catalogo-400x400_lvcpwp.png" xr:uid="{893DDDA6-C5BC-F948-AA63-B4B9B3A820B8}"/>
+    <hyperlink ref="D26" r:id="rId30" display="https://res.cloudinary.com/dkktirn06/image/upload/v1668870138/BANNERS KOA KOE/malta_del_sur_KOA_KOE_catalogo_1920x400_de1noj.png" xr:uid="{431DE40D-A5E7-2441-8E7D-8D2237643AC3}"/>
+    <hyperlink ref="C27" r:id="rId31" display="https://res.cloudinary.com/dkktirn06/image/upload/v1662524670/BANNERS KOA KOE/Pilsen-del-sur-KOA-KOE-catalogo-1920x400_svnnyg.png" xr:uid="{662AB90E-B2DC-6E42-BF20-743AD4B74E2F}"/>
+    <hyperlink ref="D27" r:id="rId32" display="https://res.cloudinary.com/dkktirn06/image/upload/v1662524068/BANNERS KOA KOE/Pilsen-KOA-KOE-catalogo-1920x400_xtmpvj.png" xr:uid="{9EAFEBF2-794B-3548-916D-536289F9A7A0}"/>
+    <hyperlink ref="C29" r:id="rId33" display="https://res.cloudinary.com/dkktirn06/image/upload/v1662526158/BANNERS KOA KOE/Quilmes-SKUS-banners-KOA-KOE-catalogo-400x400_szyuaz.png" xr:uid="{00774FA3-8748-B140-837D-A0D6B45AAC75}"/>
+    <hyperlink ref="D29" r:id="rId34" display="https://res.cloudinary.com/dkktirn06/image/upload/v1662526118/BANNERS KOA KOE/Quilmes-KOA-KOE-catalogo-1920x400_fameyv.png" xr:uid="{D9A7EDC4-8BF3-6A4F-B3FF-3F829C8D4A19}"/>
+    <hyperlink ref="C30" r:id="rId35" display="https://res.cloudinary.com/dkktirn06/image/upload/v1663856219/BANNERS KOA KOE/Stella-Artois-SKUS-banners-KOA-KOE-catalogo-400x400_t4y3va.png" xr:uid="{050498DE-4540-814C-992A-651261C9109B}"/>
+    <hyperlink ref="D30" r:id="rId36" display="https://res.cloudinary.com/dkktirn06/image/upload/v1662525249/BANNERS KOA KOE/Stella-Artois-KOA-KOE-catalogo-1920x400_zlqada.png" xr:uid="{0BB64920-78C8-724F-BCAB-3FAE351FF7A1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId37"/>

</xml_diff>